<commit_message>
added the columns needed for the gantt chart
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -14,6 +14,13 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$19</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$2:$F$19</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$I$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$I$2:$I$19</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -117,6 +124,21 @@
   </si>
   <si>
     <t xml:space="preserve"> Predecessors</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -158,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -170,11 +192,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -227,24 +264,1551 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Gantt Chart – Drone Development Project</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.5690096193007178E-2"/>
+          <c:y val="0.17911533466094223"/>
+          <c:w val="0.89968270398428651"/>
+          <c:h val="0.74212811970580939"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55.499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>59.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66.833333333333329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>66.833333333333329</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>77.166666666666657</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80.166666666666657</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2DA7-4779-AAF8-C1D11910D197}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected duration (te)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-2DA7-4779-AAF8-C1D11910D197}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>7.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2DA7-4779-AAF8-C1D11910D197}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1332681023"/>
+        <c:axId val="1332681439"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1332681023"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1332681439"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1332681439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> (Days)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1332681023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>471864</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>103970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>503620</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>21897</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H19"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Task" dataDxfId="7"/>
-    <tableColumn id="8" name=" Predecessors" dataDxfId="6"/>
-    <tableColumn id="2" name="Optimistic (a)" dataDxfId="5"/>
-    <tableColumn id="3" name="Probable (m)" dataDxfId="4"/>
-    <tableColumn id="4" name="Pessimistic (b)" dataDxfId="3"/>
-    <tableColumn id="5" name="Expected duration (te)" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K19" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K19"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Task" dataDxfId="10"/>
+    <tableColumn id="8" name=" Predecessors" dataDxfId="9"/>
+    <tableColumn id="2" name="Optimistic (a)" dataDxfId="8"/>
+    <tableColumn id="3" name="Probable (m)" dataDxfId="7"/>
+    <tableColumn id="4" name="Pessimistic (b)" dataDxfId="6"/>
+    <tableColumn id="5" name="Expected duration (te)" dataDxfId="5">
       <calculatedColumnFormula>(C2:C19 + 4*D2:D19 + E2)/6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Variance (σ²)" dataDxfId="1">
+    <tableColumn id="6" name="Variance (σ²)" dataDxfId="4">
       <calculatedColumnFormula>((E2:E19 - C2:C19)/6)^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Standard deviation (σ)" dataDxfId="0">
+    <tableColumn id="7" name="Standard deviation (σ)" dataDxfId="3">
       <calculatedColumnFormula>(E2:E19 - C2:C19)/6</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="9" name="Start" dataDxfId="1"/>
+    <tableColumn id="10" name="End" dataDxfId="0">
+      <calculatedColumnFormula>I2+F2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="Critical" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -513,10 +2077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="43" zoomScaleNormal="32" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,7 +2093,7 @@
     <col min="8" max="8" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -554,8 +2118,17 @@
       <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -583,8 +2156,18 @@
         <f t="shared" ref="H2:H19" si="2">(E2:E19 - C2:C19)/6</f>
         <v>0.83333333333333337</v>
       </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <f t="shared" ref="J2:J19" si="3">I2+F2</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -612,8 +2195,19 @@
         <f t="shared" si="2"/>
         <v>1.1666666666666667</v>
       </c>
+      <c r="I3">
+        <f>I2+F2</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" si="3"/>
+        <v>17.666666666666668</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -641,8 +2235,19 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="I4">
+        <f>I2+F2</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="3"/>
+        <v>15.5</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -670,8 +2275,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
+      <c r="I5">
+        <f>I2+F2</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="3"/>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -699,8 +2315,19 @@
         <f t="shared" si="2"/>
         <v>1.3333333333333333</v>
       </c>
+      <c r="I6" s="5">
+        <f>MAX(I3+F3,I4+F4)</f>
+        <v>17.666666666666668</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -728,8 +2355,19 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="I7" s="5">
+        <f>I5+F5</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="3"/>
+        <v>23.666666666666668</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -757,8 +2395,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
+      <c r="I8">
+        <f>MAX(I6+F6,I7+F7)</f>
+        <v>33</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="3"/>
+        <v>39.166666666666664</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -786,8 +2435,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
+      <c r="I9">
+        <f>I8+F8</f>
+        <v>39.166666666666664</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="3"/>
+        <v>43.333333333333329</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -815,8 +2475,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
+      <c r="I10">
+        <f>I8+F8</f>
+        <v>39.166666666666664</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="3"/>
+        <v>44.333333333333329</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -844,8 +2515,19 @@
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
+      <c r="I11">
+        <f>I8+F8</f>
+        <v>39.166666666666664</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="3"/>
+        <v>47.333333333333329</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -873,8 +2555,19 @@
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
+      <c r="I12">
+        <f>MAX(I9+F9,I10+F10,I11+F11)</f>
+        <v>47.333333333333329</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="3"/>
+        <v>50.333333333333329</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -902,8 +2595,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
+      <c r="I13">
+        <f>I12+F12</f>
+        <v>50.333333333333329</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="3"/>
+        <v>55.499999999999993</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -931,8 +2635,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
+      <c r="I14">
+        <f>I13+F13</f>
+        <v>55.499999999999993</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="3"/>
+        <v>59.666666666666657</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -960,8 +2675,19 @@
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
+      <c r="I15">
+        <f>I14+F14</f>
+        <v>59.666666666666657</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="3"/>
+        <v>66.833333333333329</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -989,8 +2715,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
+      <c r="I16">
+        <f>I15+F15</f>
+        <v>66.833333333333329</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -1018,8 +2755,19 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="I17">
+        <f>I15+F15</f>
+        <v>66.833333333333329</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="3"/>
+        <v>77.166666666666657</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -1047,8 +2795,19 @@
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
+      <c r="I18">
+        <f>MAX(I16+F16,I17+F17)</f>
+        <v>77.166666666666657</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="3"/>
+        <v>80.166666666666657</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1076,11 +2835,23 @@
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
+      <c r="I19">
+        <f>I18+F18</f>
+        <v>80.166666666666657</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="3"/>
+        <v>82.166666666666657</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>